<commit_message>
added a formula to the template to make sure it persisted and it did
</commit_message>
<xml_diff>
--- a/FUPLOAD_Template.xlsx
+++ b/FUPLOAD_Template.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrisd/dev-projects/recon_src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A978E54A-A96C-3B42-AFC2-17E395E1586C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909542E2-D2D5-3E44-9034-A7B44A606858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14080" yWindow="2900" windowWidth="24500" windowHeight="20640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42380" yWindow="4880" windowWidth="24500" windowHeight="20640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -444,13 +457,14 @@
   <dimension ref="A6:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18:I18"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.6640625" customWidth="1"/>
     <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
     <col min="8" max="8" width="17.5" customWidth="1"/>
     <col min="9" max="9" width="13.83203125" customWidth="1"/>
     <col min="10" max="10" width="31.83203125" customWidth="1"/>
@@ -471,6 +485,10 @@
       <c r="E10" t="s">
         <v>3</v>
       </c>
+      <c r="F10" t="str">
+        <f>"DP"&amp;TEXT(C12,"yymmdd")</f>
+        <v>DP251208</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">

</xml_diff>